<commit_message>
New ideas and lets try them
</commit_message>
<xml_diff>
--- a/src/testdata/reg.xlsx
+++ b/src/testdata/reg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="432" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="293" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Reg" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="161">
   <si>
     <t>nimi</t>
   </si>
@@ -451,13 +451,22 @@
     <t>Brauser</t>
   </si>
   <si>
+    <t>60kb</t>
+  </si>
+  <si>
     <t>1mb</t>
   </si>
   <si>
-    <t>2mb</t>
-  </si>
-  <si>
-    <t>3mb</t>
+    <t>2,7mb</t>
+  </si>
+  <si>
+    <t>Kysimuseupload</t>
+  </si>
+  <si>
+    <t>2,2mb</t>
+  </si>
+  <si>
+    <t>4,8mb</t>
   </si>
   <si>
     <t>firefox</t>
@@ -470,6 +479,9 @@
   </si>
   <si>
     <t>7914</t>
+  </si>
+  <si>
+    <t>puudu</t>
   </si>
   <si>
     <t>chrome</t>
@@ -950,7 +962,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1694,15 +1706,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.219387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1721,22 +1735,46 @@
       <c r="E1" s="0" t="s">
         <v>144</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1744,15 +1782,27 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1761,16 +1811,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
major cleaning of unnessecary stuff
</commit_message>
<xml_diff>
--- a/src/testdata/reg.xlsx
+++ b/src/testdata/reg.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="193">
   <si>
     <t>nimi</t>
   </si>
@@ -82,7 +82,7 @@
     <t>Automaaaat</t>
   </si>
   <si>
-    <t>madiskangro</t>
+    <t>tavalinetont24</t>
   </si>
   <si>
     <t>korralik3</t>
@@ -103,7 +103,7 @@
     <t>Peerfoooooo</t>
   </si>
   <si>
-    <t>testime14</t>
+    <t>puhtaloom24</t>
   </si>
   <si>
     <t>korralik4</t>
@@ -157,19 +157,19 @@
     <t>Tagasiside</t>
   </si>
   <si>
-    <t>tavalinetont33</t>
+    <t>tavalinetont34</t>
   </si>
   <si>
     <t>Toivo Tavaline</t>
   </si>
   <si>
-    <t>puhtaloom33</t>
+    <t>puhtaloom34</t>
   </si>
   <si>
     <t>Martin Loom</t>
   </si>
   <si>
-    <t>filmweird33</t>
+    <t>filmweird34</t>
   </si>
   <si>
     <t>Toomas Film</t>
@@ -214,7 +214,7 @@
     <t>Eks sa tea paremini</t>
   </si>
   <si>
-    <t>selentest20@mailinator.com</t>
+    <t>selentest21@mailinator.com</t>
   </si>
   <si>
     <t>selentest@hotmail.com</t>
@@ -232,7 +232,7 @@
     <t>Eks kaitsetoo ole kah tahtis</t>
   </si>
   <si>
-    <t>testimeauto20@mailinator.com</t>
+    <t>testimeauto21@mailinator.com</t>
   </si>
   <si>
     <t>Sa ei tea kes ma olen</t>
@@ -247,7 +247,7 @@
     <t>Indeed</t>
   </si>
   <si>
-    <t>vahekonto20@mailinator.com</t>
+    <t>vahekonto21@mailinator.com</t>
   </si>
   <si>
     <t>Password</t>
@@ -427,7 +427,7 @@
     <t>Väravaid oskab lyya, kuid kaitsa ei oska</t>
   </si>
   <si>
-    <t>Eks me kõik oleme natuke imelikud</t>
+    <t>Eks me koik oleme natuke imelikud</t>
   </si>
   <si>
     <t>Eks ta ole jah nii</t>
@@ -442,7 +442,7 @@
     <t>Oleks ma nii rahulik</t>
   </si>
   <si>
-    <t>Teda ei häiri miski</t>
+    <t>Teda ei hairi miski</t>
   </si>
   <si>
     <t>case</t>
@@ -506,6 +506,102 @@
   </si>
   <si>
     <t>7582</t>
+  </si>
+  <si>
+    <t>tavalinetont35</t>
+  </si>
+  <si>
+    <t>puhtaloom35</t>
+  </si>
+  <si>
+    <t>filmweird35</t>
+  </si>
+  <si>
+    <t>selentest22@mailinator.com</t>
+  </si>
+  <si>
+    <t>testimeauto22@mailinator.com</t>
+  </si>
+  <si>
+    <t>vahekonto22@mailinator.com</t>
+  </si>
+  <si>
+    <t>tavalinetont36</t>
+  </si>
+  <si>
+    <t>puhtaloom36</t>
+  </si>
+  <si>
+    <t>filmweird36</t>
+  </si>
+  <si>
+    <t>selentest23@mailinator.com</t>
+  </si>
+  <si>
+    <t>testimeauto23@mailinator.com</t>
+  </si>
+  <si>
+    <t>vahekonto23@mailinator.com</t>
+  </si>
+  <si>
+    <t>1523</t>
+  </si>
+  <si>
+    <t>1202</t>
+  </si>
+  <si>
+    <t>tavalinetont37</t>
+  </si>
+  <si>
+    <t>puhtaloom37</t>
+  </si>
+  <si>
+    <t>filmweird37</t>
+  </si>
+  <si>
+    <t>tavalinetont38</t>
+  </si>
+  <si>
+    <t>puhtaloom38</t>
+  </si>
+  <si>
+    <t>filmweird38</t>
+  </si>
+  <si>
+    <t>tavalinetont39</t>
+  </si>
+  <si>
+    <t>puhtaloom39</t>
+  </si>
+  <si>
+    <t>filmweird39</t>
+  </si>
+  <si>
+    <t>tavalinetont40</t>
+  </si>
+  <si>
+    <t>puhtaloom40</t>
+  </si>
+  <si>
+    <t>filmweird40</t>
+  </si>
+  <si>
+    <t>tavalinetont41</t>
+  </si>
+  <si>
+    <t>puhtaloom41</t>
+  </si>
+  <si>
+    <t>filmweird41</t>
+  </si>
+  <si>
+    <t>tavalinetont42</t>
+  </si>
+  <si>
+    <t>puhtaloom42</t>
+  </si>
+  <si>
+    <t>filmweird42</t>
   </si>
 </sst>
 </file>
@@ -642,19 +738,19 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.969387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="15.6326530612245" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="24.6785714285714" collapsed="true"/>
+    <col min="3" max="4" hidden="false" style="0" width="12.969387755102" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="16.0816326530612" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="21.2295918367347" collapsed="true"/>
+    <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -797,8 +893,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.5663265306122" collapsed="true"/>
+    <col min="2" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -818,7 +914,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet4!A2</f>
-        <v>tavalinetont33</v>
+        <v>tavalinetont42</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">Sheet6!B2</f>
@@ -835,7 +931,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet4!C2</f>
-        <v>puhtaloom33</v>
+        <v>puhtaloom42</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">Sheet6!B3</f>
@@ -852,7 +948,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet4!E2</f>
-        <v>filmweird33</v>
+        <v>filmweird42</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">Sheet6!B4</f>
@@ -885,13 +981,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.5663265306122" collapsed="true"/>
+    <col min="2" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -908,7 +1004,7 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet2!A2</f>
-        <v>tavalinetont33</v>
+        <v>tavalinetont42</v>
       </c>
       <c r="B2" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -921,7 +1017,7 @@
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet2!A3</f>
-        <v>puhtaloom33</v>
+        <v>puhtaloom42</v>
       </c>
       <c r="B3" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -934,7 +1030,7 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet2!A4</f>
-        <v>filmweird33</v>
+        <v>filmweird42</v>
       </c>
       <c r="B4" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -963,16 +1059,16 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.5612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="13.2857142857143" collapsed="true"/>
+    <col min="3" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="23.5612244897959" collapsed="true"/>
+    <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,19 +1099,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>44</v>
+        <v>190</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>46</v>
+        <v>191</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>192</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>49</v>
@@ -1046,19 +1142,19 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.3214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="28.3673469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.4387755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col min="1" max="4" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="23.5612244897959" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="19.3214285714286" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="20.8775510204082" collapsed="true"/>
+    <col min="8" max="9" hidden="false" style="0" width="28.3673469387755" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="0" width="20.4387755102041" collapsed="true"/>
+    <col min="11" max="11" hidden="false" style="0" width="20.1122448979592" collapsed="true"/>
+    <col min="12" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1099,15 +1195,15 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet4!A2</f>
-        <v>tavalinetont33</v>
+        <v>tavalinetont42</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom33</v>
+        <v>puhtaloom42</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird33</v>
+        <v>filmweird42</v>
       </c>
       <c r="D2" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1126,7 +1222,7 @@
         <v>62</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>63</v>
+        <v>170</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>64</v>
@@ -1138,15 +1234,15 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet4!C2</f>
-        <v>puhtaloom33</v>
+        <v>puhtaloom42</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird33</v>
+        <v>filmweird42</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont33</v>
+        <v>tavalinetont42</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1165,7 +1261,7 @@
         <v>68</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>69</v>
+        <v>171</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>64</v>
@@ -1177,15 +1273,15 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet4!E2</f>
-        <v>filmweird33</v>
+        <v>filmweird42</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont33</v>
+        <v>tavalinetont42</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom33</v>
+        <v>puhtaloom42</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1204,7 +1300,7 @@
         <v>73</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>64</v>
@@ -1242,15 +1338,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.5"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.4132653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.2040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1887755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.25"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col min="1" max="3" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="30.5" collapsed="true"/>
+    <col min="5" max="6" hidden="false" style="0" width="20.8775510204082" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="16.4132653061224" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="18.2040816326531" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="16.1887755102041" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="0" width="27.25" collapsed="true"/>
+    <col min="11" max="11" hidden="false" style="0" width="17.7551020408163" collapsed="true"/>
+    <col min="12" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1297,7 +1393,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet5!A2</f>
-        <v>tavalinetont33</v>
+        <v>tavalinetont42</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1340,7 +1436,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet5!A3</f>
-        <v>puhtaloom33</v>
+        <v>puhtaloom42</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1383,7 +1479,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet5!A4</f>
-        <v>filmweird33</v>
+        <v>filmweird42</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1447,11 +1543,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1275510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9540816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col min="1" max="3" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="47.1275510204082" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="34.9540816326531" collapsed="true"/>
+    <col min="7" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1477,11 +1573,11 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet6!A2</f>
-        <v>tavalinetont33</v>
+        <v>tavalinetont42</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom33</v>
+        <v>puhtaloom42</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1500,11 +1596,11 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet6!A3</f>
-        <v>puhtaloom33</v>
+        <v>puhtaloom42</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird33</v>
+        <v>filmweird42</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1523,11 +1619,11 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet6!A4</f>
-        <v>filmweird33</v>
+        <v>filmweird42</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont33</v>
+        <v>tavalinetont42</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1569,19 +1665,19 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8520408163265"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.3367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col min="1" max="2" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="3" max="4" hidden="false" style="0" width="31.0459183673469" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="26.3571428571429" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="34.5204081632653" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="12.8520408163265" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="22.3367346938776" collapsed="true"/>
+    <col min="10" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1610,11 +1706,11 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet5!A2</f>
-        <v>tavalinetont33</v>
+        <v>tavalinetont42</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom33</v>
+        <v>puhtaloom42</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1637,11 +1733,11 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet5!A3</f>
-        <v>puhtaloom33</v>
+        <v>puhtaloom42</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird33</v>
+        <v>filmweird42</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1664,11 +1760,11 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet5!A4</f>
-        <v>filmweird33</v>
+        <v>filmweird42</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont33</v>
+        <v>tavalinetont42</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1712,9 +1808,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.219387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col min="1" max="5" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="21.219387755102" collapsed="true"/>
+    <col min="7" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,10 +1891,10 @@
         <v>2</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>152</v>

</xml_diff>

<commit_message>
update excel sheet, build 207
</commit_message>
<xml_diff>
--- a/src/testdata/reg.xlsx
+++ b/src/testdata/reg.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="166">
   <si>
     <t>nimi</t>
   </si>
@@ -512,6 +512,15 @@
   </si>
   <si>
     <t>7582</t>
+  </si>
+  <si>
+    <t>tavalinetont47</t>
+  </si>
+  <si>
+    <t>puhtaloom47</t>
+  </si>
+  <si>
+    <t>filmweird47</t>
   </si>
 </sst>
 </file>
@@ -653,14 +662,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.969387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="15.6326530612245" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="24.6785714285714" collapsed="true"/>
+    <col min="3" max="4" hidden="false" style="0" width="12.969387755102" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="16.0816326530612" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="21.2295918367347" collapsed="true"/>
+    <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -803,8 +812,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.5663265306122" collapsed="true"/>
+    <col min="2" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,7 +833,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet4!A2</f>
-        <v>tavalinetont46</v>
+        <v>tavalinetont47</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">Sheet6!B2</f>
@@ -841,7 +850,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet4!C2</f>
-        <v>puhtaloom46</v>
+        <v>puhtaloom47</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">Sheet6!B3</f>
@@ -858,7 +867,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet4!E2</f>
-        <v>filmweird46</v>
+        <v>filmweird47</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">Sheet6!B4</f>
@@ -896,8 +905,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.5663265306122" collapsed="true"/>
+    <col min="2" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -914,7 +923,7 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet2!A2</f>
-        <v>tavalinetont46</v>
+        <v>tavalinetont47</v>
       </c>
       <c r="B2" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -927,7 +936,7 @@
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet2!A3</f>
-        <v>puhtaloom46</v>
+        <v>puhtaloom47</v>
       </c>
       <c r="B3" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -940,7 +949,7 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet2!A4</f>
-        <v>filmweird46</v>
+        <v>filmweird47</v>
       </c>
       <c r="B4" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -974,11 +983,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.5612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="13.2857142857143" collapsed="true"/>
+    <col min="3" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="23.5612244897959" collapsed="true"/>
+    <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1009,19 +1018,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>44</v>
+        <v>163</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>46</v>
+        <v>164</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>49</v>
@@ -1057,14 +1066,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.3214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="28.3673469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.4387755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col min="1" max="4" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="23.5612244897959" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="19.3214285714286" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="20.8775510204082" collapsed="true"/>
+    <col min="8" max="9" hidden="false" style="0" width="28.3673469387755" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="0" width="20.4387755102041" collapsed="true"/>
+    <col min="11" max="11" hidden="false" style="0" width="20.1122448979592" collapsed="true"/>
+    <col min="12" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,15 +1114,15 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet4!A2</f>
-        <v>tavalinetont46</v>
+        <v>tavalinetont47</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom46</v>
+        <v>puhtaloom47</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird46</v>
+        <v>filmweird47</v>
       </c>
       <c r="D2" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1144,15 +1153,15 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet4!C2</f>
-        <v>puhtaloom46</v>
+        <v>puhtaloom47</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird46</v>
+        <v>filmweird47</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont46</v>
+        <v>tavalinetont47</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1183,15 +1192,15 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet4!E2</f>
-        <v>filmweird46</v>
+        <v>filmweird47</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont46</v>
+        <v>tavalinetont47</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom46</v>
+        <v>puhtaloom47</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1248,15 +1257,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.5"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.4132653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.2040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1887755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.25"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col min="1" max="3" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="30.5" collapsed="true"/>
+    <col min="5" max="6" hidden="false" style="0" width="20.8775510204082" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="16.4132653061224" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="18.2040816326531" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="16.1887755102041" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="0" width="27.25" collapsed="true"/>
+    <col min="11" max="11" hidden="false" style="0" width="17.7551020408163" collapsed="true"/>
+    <col min="12" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1303,7 +1312,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet5!A2</f>
-        <v>tavalinetont46</v>
+        <v>tavalinetont47</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1346,7 +1355,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet5!A3</f>
-        <v>puhtaloom46</v>
+        <v>puhtaloom47</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1389,7 +1398,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet5!A4</f>
-        <v>filmweird46</v>
+        <v>filmweird47</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1453,11 +1462,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1275510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9540816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col min="1" max="3" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="47.1275510204082" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="34.9540816326531" collapsed="true"/>
+    <col min="7" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1483,11 +1492,11 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet6!A2</f>
-        <v>tavalinetont46</v>
+        <v>tavalinetont47</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom46</v>
+        <v>puhtaloom47</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1506,11 +1515,11 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet6!A3</f>
-        <v>puhtaloom46</v>
+        <v>puhtaloom47</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird46</v>
+        <v>filmweird47</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1529,11 +1538,11 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet6!A4</f>
-        <v>filmweird46</v>
+        <v>filmweird47</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont46</v>
+        <v>tavalinetont47</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1580,14 +1589,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8520408163265"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.3367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col min="1" max="2" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="3" max="4" hidden="false" style="0" width="31.0459183673469" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="26.3571428571429" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="34.5204081632653" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="12.8520408163265" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="22.3367346938776" collapsed="true"/>
+    <col min="10" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,11 +1625,11 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet5!A2</f>
-        <v>tavalinetont46</v>
+        <v>tavalinetont47</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom46</v>
+        <v>puhtaloom47</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1643,11 +1652,11 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet5!A3</f>
-        <v>puhtaloom46</v>
+        <v>puhtaloom47</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird46</v>
+        <v>filmweird47</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1670,11 +1679,11 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet5!A4</f>
-        <v>filmweird46</v>
+        <v>filmweird47</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont46</v>
+        <v>tavalinetont47</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1718,9 +1727,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.219387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col min="1" max="5" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="21.219387755102" collapsed="true"/>
+    <col min="7" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
update excel sheet, build 208
</commit_message>
<xml_diff>
--- a/src/testdata/reg.xlsx
+++ b/src/testdata/reg.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="169">
   <si>
     <t>nimi</t>
   </si>
@@ -521,6 +521,15 @@
   </si>
   <si>
     <t>filmweird47</t>
+  </si>
+  <si>
+    <t>tavalinetont48</t>
+  </si>
+  <si>
+    <t>puhtaloom48</t>
+  </si>
+  <si>
+    <t>filmweird48</t>
   </si>
 </sst>
 </file>
@@ -833,7 +842,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet4!A2</f>
-        <v>tavalinetont47</v>
+        <v>tavalinetont48</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">Sheet6!B2</f>
@@ -850,7 +859,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet4!C2</f>
-        <v>puhtaloom47</v>
+        <v>puhtaloom48</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">Sheet6!B3</f>
@@ -867,7 +876,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet4!E2</f>
-        <v>filmweird47</v>
+        <v>filmweird48</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">Sheet6!B4</f>
@@ -923,7 +932,7 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet2!A2</f>
-        <v>tavalinetont47</v>
+        <v>tavalinetont48</v>
       </c>
       <c r="B2" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -936,7 +945,7 @@
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet2!A3</f>
-        <v>puhtaloom47</v>
+        <v>puhtaloom48</v>
       </c>
       <c r="B3" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -949,7 +958,7 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet2!A4</f>
-        <v>filmweird47</v>
+        <v>filmweird48</v>
       </c>
       <c r="B4" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1018,19 +1027,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>49</v>
@@ -1114,15 +1123,15 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet4!A2</f>
-        <v>tavalinetont47</v>
+        <v>tavalinetont48</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom47</v>
+        <v>puhtaloom48</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird47</v>
+        <v>filmweird48</v>
       </c>
       <c r="D2" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1153,15 +1162,15 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet4!C2</f>
-        <v>puhtaloom47</v>
+        <v>puhtaloom48</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird47</v>
+        <v>filmweird48</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont47</v>
+        <v>tavalinetont48</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1192,15 +1201,15 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet4!E2</f>
-        <v>filmweird47</v>
+        <v>filmweird48</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont47</v>
+        <v>tavalinetont48</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom47</v>
+        <v>puhtaloom48</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1312,7 +1321,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet5!A2</f>
-        <v>tavalinetont47</v>
+        <v>tavalinetont48</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1355,7 +1364,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet5!A3</f>
-        <v>puhtaloom47</v>
+        <v>puhtaloom48</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1398,7 +1407,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet5!A4</f>
-        <v>filmweird47</v>
+        <v>filmweird48</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1492,11 +1501,11 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet6!A2</f>
-        <v>tavalinetont47</v>
+        <v>tavalinetont48</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom47</v>
+        <v>puhtaloom48</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1515,11 +1524,11 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet6!A3</f>
-        <v>puhtaloom47</v>
+        <v>puhtaloom48</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird47</v>
+        <v>filmweird48</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1538,11 +1547,11 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet6!A4</f>
-        <v>filmweird47</v>
+        <v>filmweird48</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont47</v>
+        <v>tavalinetont48</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1625,11 +1634,11 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet5!A2</f>
-        <v>tavalinetont47</v>
+        <v>tavalinetont48</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom47</v>
+        <v>puhtaloom48</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1652,11 +1661,11 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet5!A3</f>
-        <v>puhtaloom47</v>
+        <v>puhtaloom48</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird47</v>
+        <v>filmweird48</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1679,11 +1688,11 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet5!A4</f>
-        <v>filmweird47</v>
+        <v>filmweird48</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont47</v>
+        <v>tavalinetont48</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>

</xml_diff>

<commit_message>
tests in jenkins enviroment
</commit_message>
<xml_diff>
--- a/src/testdata/reg.xlsx
+++ b/src/testdata/reg.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="163">
   <si>
     <t>nimi</t>
   </si>
@@ -157,19 +157,19 @@
     <t>Tagasiside</t>
   </si>
   <si>
-    <t>tavalinetont46</t>
+    <t>tavalinetont50</t>
   </si>
   <si>
     <t>Toivo Tavaline</t>
   </si>
   <si>
-    <t>puhtaloom46</t>
+    <t>puhtaloom50</t>
   </si>
   <si>
     <t>Martin Loom</t>
   </si>
   <si>
-    <t>filmweird46</t>
+    <t>filmweird50</t>
   </si>
   <si>
     <t>Toomas Film</t>
@@ -512,24 +512,6 @@
   </si>
   <si>
     <t>7582</t>
-  </si>
-  <si>
-    <t>tavalinetont47</t>
-  </si>
-  <si>
-    <t>puhtaloom47</t>
-  </si>
-  <si>
-    <t>filmweird47</t>
-  </si>
-  <si>
-    <t>tavalinetont48</t>
-  </si>
-  <si>
-    <t>puhtaloom48</t>
-  </si>
-  <si>
-    <t>filmweird48</t>
   </si>
 </sst>
 </file>
@@ -671,14 +653,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="15.6326530612245" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="24.6785714285714" collapsed="true"/>
-    <col min="3" max="4" hidden="false" style="0" width="12.969387755102" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="16.0816326530612" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="0" width="21.2295918367347" collapsed="true"/>
-    <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6785714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -821,8 +803,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="11.5663265306122" collapsed="true"/>
-    <col min="2" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,7 +824,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet4!A2</f>
-        <v>tavalinetont48</v>
+        <v>tavalinetont50</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">Sheet6!B2</f>
@@ -859,7 +841,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet4!C2</f>
-        <v>puhtaloom48</v>
+        <v>puhtaloom50</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">Sheet6!B3</f>
@@ -876,7 +858,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet4!E2</f>
-        <v>filmweird48</v>
+        <v>filmweird50</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">Sheet6!B4</f>
@@ -914,8 +896,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="11.5663265306122" collapsed="true"/>
-    <col min="2" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,7 +914,7 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet2!A2</f>
-        <v>tavalinetont48</v>
+        <v>tavalinetont50</v>
       </c>
       <c r="B2" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -945,7 +927,7 @@
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet2!A3</f>
-        <v>puhtaloom48</v>
+        <v>puhtaloom50</v>
       </c>
       <c r="B3" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -958,7 +940,7 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet2!A4</f>
-        <v>filmweird48</v>
+        <v>filmweird50</v>
       </c>
       <c r="B4" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -992,11 +974,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="13.2857142857143" collapsed="true"/>
-    <col min="3" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="0" width="23.5612244897959" collapsed="true"/>
-    <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.5612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1027,19 +1009,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>166</v>
+        <v>44</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>167</v>
+        <v>46</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>168</v>
+        <v>48</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>49</v>
@@ -1075,14 +1057,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="4" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="23.5612244897959" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="19.3214285714286" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="0" width="20.8775510204082" collapsed="true"/>
-    <col min="8" max="9" hidden="false" style="0" width="28.3673469387755" collapsed="true"/>
-    <col min="10" max="10" hidden="false" style="0" width="20.4387755102041" collapsed="true"/>
-    <col min="11" max="11" hidden="false" style="0" width="20.1122448979592" collapsed="true"/>
-    <col min="12" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.3214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.8775510204082"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="28.3673469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.4387755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1123,15 +1105,15 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet4!A2</f>
-        <v>tavalinetont48</v>
+        <v>tavalinetont50</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom48</v>
+        <v>puhtaloom50</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird48</v>
+        <v>filmweird50</v>
       </c>
       <c r="D2" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1162,15 +1144,15 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet4!C2</f>
-        <v>puhtaloom48</v>
+        <v>puhtaloom50</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird48</v>
+        <v>filmweird50</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont48</v>
+        <v>tavalinetont50</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1201,15 +1183,15 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet4!E2</f>
-        <v>filmweird48</v>
+        <v>filmweird50</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont48</v>
+        <v>tavalinetont50</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom48</v>
+        <v>puhtaloom50</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1266,15 +1248,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="3" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="30.5" collapsed="true"/>
-    <col min="5" max="6" hidden="false" style="0" width="20.8775510204082" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="0" width="16.4132653061224" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="0" width="18.2040816326531" collapsed="true"/>
-    <col min="9" max="9" hidden="false" style="0" width="16.1887755102041" collapsed="true"/>
-    <col min="10" max="10" hidden="false" style="0" width="27.25" collapsed="true"/>
-    <col min="11" max="11" hidden="false" style="0" width="17.7551020408163" collapsed="true"/>
-    <col min="12" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.5"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="20.8775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.4132653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.2040816326531"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1887755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.25"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1321,7 +1303,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet5!A2</f>
-        <v>tavalinetont48</v>
+        <v>tavalinetont50</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1364,7 +1346,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet5!A3</f>
-        <v>puhtaloom48</v>
+        <v>puhtaloom50</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1407,7 +1389,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet5!A4</f>
-        <v>filmweird48</v>
+        <v>filmweird50</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1471,11 +1453,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="3" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="47.1275510204082" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="34.9540816326531" collapsed="true"/>
-    <col min="7" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1275510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1501,11 +1483,11 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet6!A2</f>
-        <v>tavalinetont48</v>
+        <v>tavalinetont50</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom48</v>
+        <v>puhtaloom50</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1524,11 +1506,11 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet6!A3</f>
-        <v>puhtaloom48</v>
+        <v>puhtaloom50</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird48</v>
+        <v>filmweird50</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1547,11 +1529,11 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet6!A4</f>
-        <v>filmweird48</v>
+        <v>filmweird50</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont48</v>
+        <v>tavalinetont50</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1598,14 +1580,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="2" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="3" max="4" hidden="false" style="0" width="31.0459183673469" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="26.3571428571429" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="34.5204081632653" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="0" width="12.8520408163265" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="9" max="9" hidden="false" style="0" width="22.3367346938776" collapsed="true"/>
-    <col min="10" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3571428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8520408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.3367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1634,11 +1616,11 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet5!A2</f>
-        <v>tavalinetont48</v>
+        <v>tavalinetont50</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom48</v>
+        <v>puhtaloom50</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1661,11 +1643,11 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet5!A3</f>
-        <v>puhtaloom48</v>
+        <v>puhtaloom50</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird48</v>
+        <v>filmweird50</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1688,11 +1670,11 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet5!A4</f>
-        <v>filmweird48</v>
+        <v>filmweird50</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont48</v>
+        <v>tavalinetont50</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1736,9 +1718,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="5" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="21.219387755102" collapsed="true"/>
-    <col min="7" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.219387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
update excel sheet, build 212
</commit_message>
<xml_diff>
--- a/src/testdata/reg.xlsx
+++ b/src/testdata/reg.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="187">
   <si>
     <t>nimi</t>
   </si>
@@ -512,6 +512,78 @@
   </si>
   <si>
     <t>7582</t>
+  </si>
+  <si>
+    <t>tavalinetont51</t>
+  </si>
+  <si>
+    <t>puhtaloom51</t>
+  </si>
+  <si>
+    <t>filmweird51</t>
+  </si>
+  <si>
+    <t>selentest24@mailinator.com</t>
+  </si>
+  <si>
+    <t>testimeauto24@mailinator.com</t>
+  </si>
+  <si>
+    <t>vahekonto24@mailinator.com</t>
+  </si>
+  <si>
+    <t>1027</t>
+  </si>
+  <si>
+    <t>1090</t>
+  </si>
+  <si>
+    <t>1067</t>
+  </si>
+  <si>
+    <t>1782</t>
+  </si>
+  <si>
+    <t>7262</t>
+  </si>
+  <si>
+    <t>7742</t>
+  </si>
+  <si>
+    <t>tavalinetont52</t>
+  </si>
+  <si>
+    <t>puhtaloom52</t>
+  </si>
+  <si>
+    <t>filmweird52</t>
+  </si>
+  <si>
+    <t>selentest25@mailinator.com</t>
+  </si>
+  <si>
+    <t>testimeauto25@mailinator.com</t>
+  </si>
+  <si>
+    <t>vahekonto25@mailinator.com</t>
+  </si>
+  <si>
+    <t>1356</t>
+  </si>
+  <si>
+    <t>1309</t>
+  </si>
+  <si>
+    <t>1254</t>
+  </si>
+  <si>
+    <t>2309</t>
+  </si>
+  <si>
+    <t>6956</t>
+  </si>
+  <si>
+    <t>8025</t>
   </si>
 </sst>
 </file>
@@ -653,14 +725,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.969387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="15.6326530612245" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="24.6785714285714" collapsed="true"/>
+    <col min="3" max="4" hidden="false" style="0" width="12.969387755102" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="16.0816326530612" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="21.2295918367347" collapsed="true"/>
+    <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -803,8 +875,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.5663265306122" collapsed="true"/>
+    <col min="2" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,7 +896,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet4!A2</f>
-        <v>tavalinetont50</v>
+        <v>tavalinetont52</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">Sheet6!B2</f>
@@ -841,7 +913,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet4!C2</f>
-        <v>puhtaloom50</v>
+        <v>puhtaloom52</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">Sheet6!B3</f>
@@ -858,7 +930,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet4!E2</f>
-        <v>filmweird50</v>
+        <v>filmweird52</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">Sheet6!B4</f>
@@ -896,8 +968,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.5663265306122" collapsed="true"/>
+    <col min="2" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -914,7 +986,7 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet2!A2</f>
-        <v>tavalinetont50</v>
+        <v>tavalinetont52</v>
       </c>
       <c r="B2" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -927,7 +999,7 @@
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet2!A3</f>
-        <v>puhtaloom50</v>
+        <v>puhtaloom52</v>
       </c>
       <c r="B3" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -940,7 +1012,7 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet2!A4</f>
-        <v>filmweird50</v>
+        <v>filmweird52</v>
       </c>
       <c r="B4" s="2" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -974,11 +1046,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.5612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="13.2857142857143" collapsed="true"/>
+    <col min="3" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="23.5612244897959" collapsed="true"/>
+    <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1009,19 +1081,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>44</v>
+        <v>175</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>46</v>
+        <v>176</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>177</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>49</v>
@@ -1057,14 +1129,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.3214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="28.3673469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.4387755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col min="1" max="4" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="23.5612244897959" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="19.3214285714286" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="20.8775510204082" collapsed="true"/>
+    <col min="8" max="9" hidden="false" style="0" width="28.3673469387755" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="0" width="20.4387755102041" collapsed="true"/>
+    <col min="11" max="11" hidden="false" style="0" width="20.1122448979592" collapsed="true"/>
+    <col min="12" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,15 +1177,15 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet4!A2</f>
-        <v>tavalinetont50</v>
+        <v>tavalinetont52</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom50</v>
+        <v>puhtaloom52</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird50</v>
+        <v>filmweird52</v>
       </c>
       <c r="D2" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1132,7 +1204,7 @@
         <v>62</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>63</v>
+        <v>178</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>64</v>
@@ -1144,15 +1216,15 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet4!C2</f>
-        <v>puhtaloom50</v>
+        <v>puhtaloom52</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird50</v>
+        <v>filmweird52</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont50</v>
+        <v>tavalinetont52</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1171,7 +1243,7 @@
         <v>68</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>69</v>
+        <v>179</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>64</v>
@@ -1183,15 +1255,15 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet4!E2</f>
-        <v>filmweird50</v>
+        <v>filmweird52</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont50</v>
+        <v>tavalinetont52</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom50</v>
+        <v>puhtaloom52</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">Sheet4!G2</f>
@@ -1210,7 +1282,7 @@
         <v>73</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>74</v>
+        <v>180</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>64</v>
@@ -1248,15 +1320,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.5"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.4132653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.2040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1887755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.25"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col min="1" max="3" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="30.5" collapsed="true"/>
+    <col min="5" max="6" hidden="false" style="0" width="20.8775510204082" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="16.4132653061224" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="18.2040816326531" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="16.1887755102041" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="0" width="27.25" collapsed="true"/>
+    <col min="11" max="11" hidden="false" style="0" width="17.7551020408163" collapsed="true"/>
+    <col min="12" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1303,7 +1375,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet5!A2</f>
-        <v>tavalinetont50</v>
+        <v>tavalinetont52</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1346,7 +1418,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet5!A3</f>
-        <v>puhtaloom50</v>
+        <v>puhtaloom52</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1389,7 +1461,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet5!A4</f>
-        <v>filmweird50</v>
+        <v>filmweird52</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1453,11 +1525,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1275510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9540816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col min="1" max="3" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="47.1275510204082" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="34.9540816326531" collapsed="true"/>
+    <col min="7" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1483,11 +1555,11 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet6!A2</f>
-        <v>tavalinetont50</v>
+        <v>tavalinetont52</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom50</v>
+        <v>puhtaloom52</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1506,11 +1578,11 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet6!A3</f>
-        <v>puhtaloom50</v>
+        <v>puhtaloom52</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird50</v>
+        <v>filmweird52</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1529,11 +1601,11 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet6!A4</f>
-        <v>filmweird50</v>
+        <v>filmweird52</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont50</v>
+        <v>tavalinetont52</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1580,14 +1652,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8520408163265"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.3367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col min="1" max="2" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="3" max="4" hidden="false" style="0" width="31.0459183673469" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="26.3571428571429" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="34.5204081632653" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="12.8520408163265" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="22.3367346938776" collapsed="true"/>
+    <col min="10" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,11 +1688,11 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">Sheet5!A2</f>
-        <v>tavalinetont50</v>
+        <v>tavalinetont52</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">A3</f>
-        <v>puhtaloom50</v>
+        <v>puhtaloom52</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">Sheet5!D2</f>
@@ -1643,11 +1715,11 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">Sheet5!A3</f>
-        <v>puhtaloom50</v>
+        <v>puhtaloom52</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">A4</f>
-        <v>filmweird50</v>
+        <v>filmweird52</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">Sheet5!D3</f>
@@ -1670,11 +1742,11 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">Sheet5!A4</f>
-        <v>filmweird50</v>
+        <v>filmweird52</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">A2</f>
-        <v>tavalinetont50</v>
+        <v>tavalinetont52</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">Sheet5!D4</f>
@@ -1718,9 +1790,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.219387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col min="1" max="5" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="21.219387755102" collapsed="true"/>
+    <col min="7" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1760,25 +1832,25 @@
         <v>148</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>152</v>
+        <v>181</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>152</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1789,25 +1861,25 @@
         <v>153</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="F3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>